<commit_message>
updated files as of 10:58 am
</commit_message>
<xml_diff>
--- a/Svedka Analysis Regression Summaries.xlsx
+++ b/Svedka Analysis Regression Summaries.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1140" windowWidth="24960" windowHeight="13760" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="640" yWindow="1140" windowWidth="24960" windowHeight="13760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Q2RegSummary" sheetId="3" r:id="rId1"/>
-    <sheet name="Q3RegSummary" sheetId="4" r:id="rId2"/>
+    <sheet name="Q3RegSummary" sheetId="8" r:id="rId2"/>
     <sheet name="Q4RegSummary" sheetId="1" r:id="rId3"/>
-    <sheet name="Q5RegSummary" sheetId="5" r:id="rId4"/>
+    <sheet name="Q5RegSummary" sheetId="7" r:id="rId4"/>
     <sheet name="Q6RegSummary" sheetId="6" r:id="rId5"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId6"/>
   </sheets>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="19">
   <si>
     <t>term</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Firstintro</t>
+  </si>
+  <si>
+    <t>LnPrice</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -566,11 +569,6 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -598,16 +596,16 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>5.1205311660820598E-3</v>
+        <v>-0.11736535028180101</v>
       </c>
       <c r="D2">
-        <v>1.90895554966375E-2</v>
+        <v>9.8395868188021304E-2</v>
       </c>
       <c r="E2">
-        <v>0.26823731788747002</v>
+        <v>-1.1927873847053401</v>
       </c>
       <c r="F2">
-        <v>0.78873099371032596</v>
+        <v>0.23404845575907099</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -615,19 +613,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C3">
-        <v>3.5417918749696298E-4</v>
+        <v>3.6774462363971298E-2</v>
       </c>
       <c r="D3">
-        <v>2.6029978726742299E-4</v>
+        <v>2.5379123556186999E-2</v>
       </c>
       <c r="E3">
-        <v>1.3606587666285399</v>
+        <v>1.4490044261204</v>
       </c>
       <c r="F3">
-        <v>0.174809007557407</v>
+        <v>0.14855067433341401</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -638,16 +636,16 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>1.5400533403330899E-2</v>
+        <v>1.4776084997315199E-2</v>
       </c>
       <c r="D4">
-        <v>4.4310201275025501E-3</v>
+        <v>4.6001787421577796E-3</v>
       </c>
       <c r="E4">
-        <v>3.47561802027088</v>
+        <v>3.21206757944024</v>
       </c>
       <c r="F4">
-        <v>5.9777927219314703E-4</v>
+        <v>1.4851890583199999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -658,16 +656,16 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>-1.17752760610654E-2</v>
+        <v>-1.262205486868E-2</v>
       </c>
       <c r="D5">
-        <v>5.9667927056446801E-3</v>
+        <v>5.7857043577503302E-3</v>
       </c>
       <c r="E5">
-        <v>-1.97346826711875</v>
+        <v>-2.1815934738822098</v>
       </c>
       <c r="F5">
-        <v>4.95093097031091E-2</v>
+        <v>3.00423405364139E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -678,16 +676,16 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>-5.9870832829268398E-3</v>
+        <v>-5.7637188827885204E-3</v>
       </c>
       <c r="D6">
-        <v>5.1876297556668199E-3</v>
+        <v>5.1584593239443303E-3</v>
       </c>
       <c r="E6">
-        <v>-1.1541076686104501</v>
+        <v>-1.1173333975969799</v>
       </c>
       <c r="F6">
-        <v>0.24952396517608699</v>
+        <v>0.26489119983752701</v>
       </c>
     </row>
   </sheetData>
@@ -931,16 +929,16 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>-2.0330320333849201</v>
+        <v>-1.9702928229901899</v>
       </c>
       <c r="D2">
-        <v>0.58206514236254103</v>
+        <v>0.54531605123090998</v>
       </c>
       <c r="E2">
-        <v>-3.4927912452085002</v>
+        <v>-3.6131209021681299</v>
       </c>
       <c r="F2">
-        <v>5.6260334155117098E-4</v>
+        <v>3.6385163339560002E-4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -948,19 +946,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C3">
-        <v>-1.0651582770238E-4</v>
+        <v>-5.7904941437127997E-3</v>
       </c>
       <c r="D3">
-        <v>2.8672525123327202E-4</v>
+        <v>2.7748336049512701E-2</v>
       </c>
       <c r="E3">
-        <v>-0.37149092116662402</v>
+        <v>-0.20867896847510201</v>
       </c>
       <c r="F3">
-        <v>0.71057799680297595</v>
+        <v>0.83486415545924098</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -971,16 +969,16 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>1.8694725070678399E-2</v>
+        <v>1.8269009269862801E-2</v>
       </c>
       <c r="D4">
-        <v>4.43802392355568E-3</v>
+        <v>4.6180295795582096E-3</v>
       </c>
       <c r="E4">
-        <v>4.2123984441481896</v>
+        <v>3.9560182443895302</v>
       </c>
       <c r="F4" s="1">
-        <v>3.4991568294888603E-5</v>
+        <v>9.8633033965413004E-5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -991,16 +989,16 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>-7.0155636666933098E-3</v>
+        <v>-6.7009009023669399E-3</v>
       </c>
       <c r="D5">
-        <v>5.9964843076121101E-3</v>
+        <v>5.9209043840908002E-3</v>
       </c>
       <c r="E5">
-        <v>-1.1699461395717401</v>
+        <v>-1.13173604363076</v>
       </c>
       <c r="F5">
-        <v>0.243106463487682</v>
+        <v>0.25880030987978397</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1011,16 +1009,16 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>3.9467704901347701E-3</v>
+        <v>3.5672735736858598E-3</v>
       </c>
       <c r="D6">
-        <v>5.8159107219699401E-3</v>
+        <v>5.7301758659404102E-3</v>
       </c>
       <c r="E6">
-        <v>0.67861607215283004</v>
+        <v>0.62254172596854696</v>
       </c>
       <c r="F6">
-        <v>0.49799176678588702</v>
+        <v>0.53413768327368305</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1031,16 +1029,16 @@
         <v>16</v>
       </c>
       <c r="C7" s="1">
-        <v>3.2701527654480802E-5</v>
+        <v>3.1969885502778801E-5</v>
       </c>
       <c r="D7" s="1">
-        <v>9.3342417433151706E-6</v>
+        <v>9.2606167482020302E-6</v>
       </c>
       <c r="E7">
-        <v>3.5033941217453899</v>
+        <v>3.4522415052956199</v>
       </c>
       <c r="F7">
-        <v>5.4166097246477495E-4</v>
+        <v>6.4989707420020498E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1052,7 +1050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>